<commit_message>
report: Gantt diagram update
</commit_message>
<xml_diff>
--- a/latex/report/figures/planning.xlsx
+++ b/latex/report/figures/planning.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="18" count="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="26" count="33">
   <si>
     <t>Name</t>
   </si>
@@ -26,46 +26,70 @@
     <t>Duration</t>
   </si>
   <si>
-    <t>Scientific paper</t>
-  </si>
-  <si>
-    <t>89 days</t>
-  </si>
-  <si>
-    <t>Results &amp; Conclusion</t>
-  </si>
-  <si>
-    <t>23 days</t>
-  </si>
-  <si>
-    <t>Materials and methods</t>
-  </si>
-  <si>
-    <t>54 days</t>
+    <t>Progress %</t>
+  </si>
+  <si>
+    <t>Project Report Delivery</t>
+  </si>
+  <si>
+    <t>1 day</t>
+  </si>
+  <si>
+    <t>Writting the document</t>
+  </si>
+  <si>
+    <t>132.88 days</t>
+  </si>
+  <si>
+    <t>Finalization - Results &amp; Conclusion</t>
+  </si>
+  <si>
+    <t>24 days</t>
+  </si>
+  <si>
+    <t>Document revision</t>
+  </si>
+  <si>
+    <t>11 days</t>
+  </si>
+  <si>
+    <t>Project Architecture </t>
+  </si>
+  <si>
+    <t>58.88 days</t>
+  </si>
+  <si>
+    <t>Project implementation</t>
+  </si>
+  <si>
+    <t>91 days</t>
+  </si>
+  <si>
+    <t>Choosen Machine Learning Algorithms</t>
+  </si>
+  <si>
+    <t>0 days</t>
+  </si>
+  <si>
+    <t>Dataset integration</t>
+  </si>
+  <si>
+    <t>Learning Model</t>
+  </si>
+  <si>
+    <t>Working Model</t>
   </si>
   <si>
     <t>Project Testing</t>
   </si>
   <si>
-    <t>40 days</t>
-  </si>
-  <si>
-    <t>Project implementation</t>
-  </si>
-  <si>
-    <t>50 days</t>
-  </si>
-  <si>
-    <t>Project Architecture </t>
-  </si>
-  <si>
-    <t>17 days</t>
-  </si>
-  <si>
-    <t>EV data collection</t>
-  </si>
-  <si>
-    <t>11 days</t>
+    <t>26 days</t>
+  </si>
+  <si>
+    <t>Passing With VED dataset</t>
+  </si>
+  <si>
+    <t>Passing with Emobpy dataset</t>
   </si>
 </sst>
 </file>
@@ -101,7 +125,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="8">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -207,8 +231,22 @@
         <color rgb="FFE0E0E0"/>
       </bottom>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFE0E0E0"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFE0E0E0"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFE0E0E0"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFE0E0E0"/>
+      </bottom>
+    </border>
   </borders>
-  <cellStyleXfs count="5">
+  <cellStyleXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1">
       <alignment horizontal="general" vertical="bottom" wrapText="0"/>
@@ -222,8 +260,11 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4">
       <alignment horizontal="general" vertical="bottom" wrapText="0"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5">
+      <alignment horizontal="general" vertical="bottom" wrapText="0"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="general" vertical="bottom" wrapText="0"/>
@@ -240,22 +281,26 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="4">
       <alignment horizontal="general" vertical="bottom" wrapText="0"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyAlignment="1">
-      <alignment horizontal="general" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="5">
+      <alignment horizontal="general" vertical="bottom" wrapText="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyAlignment="1">
+      <alignment horizontal="general" vertical="bottom" wrapText="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="bottom" wrapText="0"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyAlignment="1">
       <alignment horizontal="left" indent="1" vertical="bottom" wrapText="0"/>
     </xf>
   </cellXfs>
-  <cellStyles count="5">
+  <cellStyles count="6">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="treeGridGanttContainer_gridcontrolcolumn1" xfId="1"/>
     <cellStyle name="treeGridGanttContainer_gridcontrolcolumn2" xfId="2"/>
     <cellStyle name="treeGridGanttContainer_gridcontrolcolumn3" xfId="3"/>
     <cellStyle name="treeGridGanttContainer_gridcontrolcolumn4" xfId="4"/>
+    <cellStyle name="treeGridGanttContainer_gridcontrolcolumn5" xfId="5"/>
   </cellStyles>
 </styleSheet>
 </file>
@@ -269,136 +314,266 @@
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <cols>
-    <col min="1" max="1" width="33.714285714285715" customWidth="1"/>
-    <col min="2" max="2" width="21.424285714285713" customWidth="1"/>
-    <col min="3" max="3" width="21.424285714285713" customWidth="1"/>
-    <col min="4" max="4" width="21.424285714285713" customWidth="1"/>
+    <col min="1" max="1" width="48.114285714285714" customWidth="1"/>
+    <col min="2" max="2" width="18.36428571428571" customWidth="1"/>
+    <col min="3" max="3" width="16.264285714285716" customWidth="1"/>
+    <col min="4" max="4" width="15.944285714285714" customWidth="1"/>
+    <col min="5" max="5" width="22.604285714285716" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
-      <c r="A1" t="s" s="6">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s" s="6">
+    <row r="1" spans="1:5">
+      <c r="A1" t="s" s="7">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s" s="7">
         <v>1</v>
       </c>
-      <c r="C1" t="s" s="6">
+      <c r="C1" t="s" s="7">
         <v>2</v>
       </c>
-      <c r="D1" t="s" s="6">
+      <c r="D1" t="s" s="7">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:4">
-      <c r="A2" t="s" s="7">
+      <c r="E1" t="s" s="7">
         <v>4</v>
       </c>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" t="s" s="8">
+        <v>5</v>
+      </c>
       <c r="B2" t="n" s="3">
-        <v>44680.333333333336</v>
+        <v>44635.333333333336</v>
       </c>
       <c r="C2" t="n" s="4">
-        <v>44804.708333333336</v>
+        <v>44635.708333333336</v>
       </c>
       <c r="D2" t="s" s="5">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" outlineLevel="1">
+        <v>6</v>
+      </c>
+      <c r="E2" t="n" s="6">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
       <c r="A3" t="s" s="8">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B3" t="n" s="3">
-        <v>44742.333333333336</v>
+        <v>44635.333333333336</v>
       </c>
       <c r="C3" t="n" s="4">
+        <v>44819.708333333336</v>
+      </c>
+      <c r="D3" t="s" s="5">
+        <v>8</v>
+      </c>
+      <c r="E3" t="n" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" outlineLevel="1">
+      <c r="A4" t="s" s="9">
+        <v>7</v>
+      </c>
+      <c r="B4" t="n" s="3">
+        <v>44635.333333333336</v>
+      </c>
+      <c r="C4" t="n" s="4">
+        <v>44819.668333333335</v>
+      </c>
+      <c r="D4" t="s" s="5">
+        <v>8</v>
+      </c>
+      <c r="E4" t="n" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" outlineLevel="1">
+      <c r="A5" t="s" s="9">
+        <v>9</v>
+      </c>
+      <c r="B5" t="n" s="3">
+        <v>44774.333333333336</v>
+      </c>
+      <c r="C5" t="n" s="4">
+        <v>44805.708333333336</v>
+      </c>
+      <c r="D5" t="s" s="5">
+        <v>10</v>
+      </c>
+      <c r="E5" t="n" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" outlineLevel="1">
+      <c r="A6" t="s" s="9">
+        <v>11</v>
+      </c>
+      <c r="B6" t="n" s="3">
+        <v>44805.333333333336</v>
+      </c>
+      <c r="C6" t="n" s="4">
+        <v>44819.708333333336</v>
+      </c>
+      <c r="D6" t="s" s="5">
+        <v>12</v>
+      </c>
+      <c r="E6" t="n" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
+      <c r="A7" t="s" s="8">
+        <v>13</v>
+      </c>
+      <c r="B7" t="n" s="3">
+        <v>44636.333333333336</v>
+      </c>
+      <c r="C7" t="n" s="4">
+        <v>44718.666666666664</v>
+      </c>
+      <c r="D7" t="s" s="5">
+        <v>14</v>
+      </c>
+      <c r="E7" t="n" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
+      <c r="A8" t="s" s="8">
+        <v>15</v>
+      </c>
+      <c r="B8" t="n" s="3">
+        <v>44648.333333333336</v>
+      </c>
+      <c r="C8" t="n" s="4">
         <v>44774.708333333336</v>
       </c>
-      <c r="D3" t="s" s="5">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" outlineLevel="1">
-      <c r="A4" t="s" s="8">
-        <v>4</v>
-      </c>
-      <c r="B4" t="n" s="3">
-        <v>44680.333333333336</v>
-      </c>
-      <c r="C4" t="n" s="4">
-        <v>44804.708333333336</v>
-      </c>
-      <c r="D4" t="s" s="5">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" outlineLevel="1">
-      <c r="A5" t="s" s="8">
-        <v>8</v>
-      </c>
-      <c r="B5" t="n" s="3">
-        <v>44713.333333333336</v>
-      </c>
-      <c r="C5" t="n" s="4">
-        <v>44788.708333333336</v>
-      </c>
-      <c r="D5" t="s" s="5">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4">
-      <c r="A6" t="s" s="7">
-        <v>10</v>
-      </c>
-      <c r="B6" t="n" s="3">
-        <v>44690.333333333336</v>
-      </c>
-      <c r="C6" t="n" s="4">
-        <v>44743.708333333336</v>
-      </c>
-      <c r="D6" t="s" s="5">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4">
-      <c r="A7" t="s" s="7">
-        <v>12</v>
-      </c>
-      <c r="B7" t="n" s="3">
-        <v>44673.333333333336</v>
-      </c>
-      <c r="C7" t="n" s="4">
-        <v>44742.708333333336</v>
-      </c>
-      <c r="D7" t="s" s="5">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4">
-      <c r="A8" t="s" s="7">
-        <v>14</v>
-      </c>
-      <c r="B8" t="n" s="3">
-        <v>44651.333333333336</v>
-      </c>
-      <c r="C8" t="n" s="4">
-        <v>44673.708333333336</v>
-      </c>
       <c r="D8" t="s" s="5">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4">
-      <c r="A9" t="s" s="7">
         <v>16</v>
       </c>
+      <c r="E8" t="n" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5">
+      <c r="A9" t="s" s="8">
+        <v>17</v>
+      </c>
       <c r="B9" t="n" s="3">
-        <v>44651.333333333336</v>
+        <v>44662.708333333336</v>
       </c>
       <c r="C9" t="n" s="4">
-        <v>44665.708333333336</v>
+        <v>44662.708333333336</v>
       </c>
       <c r="D9" t="s" s="5">
-        <v>17</v>
+        <v>18</v>
+      </c>
+      <c r="E9" t="n" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5">
+      <c r="A10" t="s" s="8">
+        <v>19</v>
+      </c>
+      <c r="B10" t="n" s="3">
+        <v>44676.708333333336</v>
+      </c>
+      <c r="C10" t="n" s="4">
+        <v>44676.708333333336</v>
+      </c>
+      <c r="D10" t="s" s="5">
+        <v>18</v>
+      </c>
+      <c r="E10" t="n" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5">
+      <c r="A11" t="s" s="8">
+        <v>20</v>
+      </c>
+      <c r="B11" t="n" s="3">
+        <v>44697.708333333336</v>
+      </c>
+      <c r="C11" t="n" s="4">
+        <v>44697.708333333336</v>
+      </c>
+      <c r="D11" t="s" s="5">
+        <v>18</v>
+      </c>
+      <c r="E11" t="n" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5">
+      <c r="A12" t="s" s="8">
+        <v>21</v>
+      </c>
+      <c r="B12" t="n" s="3">
+        <v>44725.708333333336</v>
+      </c>
+      <c r="C12" t="n" s="4">
+        <v>44725.708333333336</v>
+      </c>
+      <c r="D12" t="s" s="5">
+        <v>18</v>
+      </c>
+      <c r="E12" t="n" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5">
+      <c r="A13" t="s" s="8">
+        <v>22</v>
+      </c>
+      <c r="B13" t="n" s="3">
+        <v>44739.333333333336</v>
+      </c>
+      <c r="C13" t="n" s="4">
+        <v>44774.708333333336</v>
+      </c>
+      <c r="D13" t="s" s="5">
+        <v>23</v>
+      </c>
+      <c r="E13" t="n" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5">
+      <c r="A14" t="s" s="8">
+        <v>24</v>
+      </c>
+      <c r="B14" t="n" s="3">
+        <v>44757.708333333336</v>
+      </c>
+      <c r="C14" t="n" s="4">
+        <v>44757.708333333336</v>
+      </c>
+      <c r="D14" t="s" s="5">
+        <v>18</v>
+      </c>
+      <c r="E14" t="n" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5">
+      <c r="A15" t="s" s="8">
+        <v>25</v>
+      </c>
+      <c r="B15" t="n" s="3">
+        <v>44774.708333333336</v>
+      </c>
+      <c r="C15" t="n" s="4">
+        <v>44774.708333333336</v>
+      </c>
+      <c r="D15" t="s" s="5">
+        <v>18</v>
+      </c>
+      <c r="E15" t="n" s="6">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>